<commit_message>
Fixed typo in xlsx file and in document tables
</commit_message>
<xml_diff>
--- a/doc/apartments.xlsx
+++ b/doc/apartments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="0" windowWidth="20440" windowHeight="23040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="21500"/>
   </bookViews>
   <sheets>
     <sheet name="apartments" sheetId="3" r:id="rId1"/>
@@ -246,7 +246,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,6 +274,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,50 +484,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="26" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -521,11 +499,53 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="187">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="6" builtinId="8" hidden="1"/>
@@ -608,6 +628,16 @@
     <cellStyle name="Гиперссылка" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="5" builtinId="9" hidden="1"/>
@@ -691,6 +721,16 @@
     <cellStyle name="Открывавшаяся гиперссылка" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Процентный" xfId="26" builtinId="5"/>
     <cellStyle name="Стиль 1" xfId="1"/>
   </cellStyles>
@@ -972,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -990,6 +1030,7 @@
     <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
+    <col min="23" max="23" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,10 +1068,10 @@
       <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="22"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -1055,22 +1096,22 @@
       <c r="G3" s="6">
         <v>0.2</v>
       </c>
-      <c r="H3" s="23">
-        <f>GEOMEAN(B3:G3)/SUM($J$3:$J$8)</f>
+      <c r="H3" s="34">
+        <f t="shared" ref="H3:H8" si="0">GEOMEAN(B3:G3)/SUM($J$3:$J$8)</f>
         <v>0.11598237204722957</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="38">
-        <f>GEOMEAN(B3:G3)</f>
+      <c r="I3" s="34"/>
+      <c r="J3" s="24">
+        <f t="shared" ref="J3:J8" si="1">GEOMEAN(B3:G3)</f>
         <v>0.81818882300002704</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="R3" s="35"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="R3" s="21"/>
     </row>
     <row r="4" spans="1:34" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1094,17 +1135,17 @@
       <c r="G4" s="6">
         <v>0.5</v>
       </c>
-      <c r="H4" s="24">
-        <f>GEOMEAN(B4:G4)/SUM($J$3:$J$8)</f>
+      <c r="H4" s="35">
+        <f t="shared" si="0"/>
         <v>0.27430369726673426</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="38">
-        <f>GEOMEAN(B4:G4)</f>
+      <c r="I4" s="36"/>
+      <c r="J4" s="24">
+        <f t="shared" si="1"/>
         <v>1.9350545712225413</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="35"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -1128,17 +1169,17 @@
       <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="23">
-        <f>GEOMEAN(B5:G5)/SUM($J$3:$J$8)</f>
+      <c r="H5" s="34">
+        <f t="shared" si="0"/>
         <v>0.14175501887444597</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="38">
-        <f>GEOMEAN(B5:G5)</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="35"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="24"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -1162,17 +1203,17 @@
       <c r="G6" s="6">
         <v>0.2</v>
       </c>
-      <c r="H6" s="23">
-        <f>GEOMEAN(B6:G6)/SUM($J$3:$J$8)</f>
+      <c r="H6" s="34">
+        <f t="shared" si="0"/>
         <v>3.9291958666538389E-2</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="38">
-        <f>GEOMEAN(B6:G6)</f>
+      <c r="I6" s="34"/>
+      <c r="J6" s="24">
+        <f t="shared" si="1"/>
         <v>0.27718213420958115</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:34" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
@@ -1196,17 +1237,17 @@
       <c r="G7" s="6">
         <v>3</v>
       </c>
-      <c r="H7" s="23">
-        <f>GEOMEAN(B7:G7)/SUM($J$3:$J$8)</f>
+      <c r="H7" s="34">
+        <f t="shared" si="0"/>
         <v>0.20210869218483324</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="38">
-        <f>GEOMEAN(B7:G7)</f>
+      <c r="I7" s="34"/>
+      <c r="J7" s="24">
+        <f t="shared" si="1"/>
         <v>1.4257603983943821</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="35"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
@@ -1230,17 +1271,17 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="23">
-        <f>GEOMEAN(B8:G8)/SUM($J$3:$J$8)</f>
+      <c r="H8" s="34">
+        <f t="shared" si="0"/>
         <v>0.22655826096021861</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="38">
-        <f>GEOMEAN(B8:G8)</f>
+      <c r="I8" s="34"/>
+      <c r="J8" s="24">
+        <f t="shared" si="1"/>
         <v>1.5982380218994845</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="35"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
@@ -1264,11 +1305,14 @@
       <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="37">
         <v>8.1631300000000007</v>
       </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="23">
+        <f>SUM(H3:I8)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -1292,11 +1336,11 @@
       <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="37">
         <f xml:space="preserve"> (H9 - COUNT(B3:B8)) / (COUNT(B3:B8) - 1)</f>
         <v>0.43262600000000012</v>
       </c>
-      <c r="I10" s="39"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -1320,37 +1364,37 @@
       <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="38">
         <f>H10/G47</f>
         <v>0.34889193548387104</v>
       </c>
-      <c r="I11" s="27"/>
+      <c r="I11" s="39"/>
     </row>
     <row r="14" spans="1:34" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="21"/>
-      <c r="Q14" s="32" t="s">
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="27"/>
+      <c r="Q14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:34" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
@@ -1389,16 +1433,16 @@
       <c r="O15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="33" t="s">
+      <c r="Q15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="R15" s="33" t="s">
+      <c r="R15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="T15" s="33" t="s">
+      <c r="T15" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1451,31 +1495,31 @@
       </c>
       <c r="Q16" s="1">
         <f>($F16*$H$3+$O16*$H$4+$F26*$H$6+$O26*$H$7+$F36*$H$5+$O36*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.22808444509360706</v>
+        <v>0.22544203099177151</v>
       </c>
       <c r="R16" s="1">
         <f>($F17*$H$3+$O17*$H$4+$F27*$H$6+$O27*$H$7+$F37*$H$5+$O37*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.23566820040799744</v>
+        <v>0.21213101206291404</v>
       </c>
       <c r="S16" s="1">
         <f>($F18*$H$3+$O18*$H$4+$F28*$H$6+$O28*$H$7+$F38*$H$5+$O38*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.17515634621254469</v>
+        <v>0.19767963186356491</v>
       </c>
       <c r="T16" s="1">
         <f>($F19*$H$3+$O19*$H$4+$F29*$H$6+$O29*$H$7+$F39*$H$5+$O39*$H$8)/  SUM($H$3:$I$8)</f>
-        <v>0.36378812365520208</v>
-      </c>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="37"/>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="37"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="37"/>
-      <c r="AE16" s="37"/>
-      <c r="AF16" s="37"/>
-      <c r="AG16" s="37"/>
-      <c r="AH16" s="37"/>
+        <v>0.36474732508174962</v>
+      </c>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="23"/>
+      <c r="AG16" s="23"/>
+      <c r="AH16" s="23"/>
     </row>
     <row r="17" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
@@ -1524,17 +1568,17 @@
         <f>GEOMEAN(K17:N17)</f>
         <v>0.26269098944241581</v>
       </c>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="37"/>
-      <c r="AB17" s="37"/>
-      <c r="AC17" s="37"/>
-      <c r="AD17" s="37"/>
-      <c r="AE17" s="37"/>
-      <c r="AF17" s="37"/>
-      <c r="AG17" s="37"/>
-      <c r="AH17" s="37"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="23"/>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="23"/>
+      <c r="AH17" s="23"/>
     </row>
     <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
@@ -1583,17 +1627,17 @@
         <f>GEOMEAN(K18:N18)</f>
         <v>1.7320508075688774</v>
       </c>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="37"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="23"/>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="23"/>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="23"/>
+      <c r="AH18" s="23"/>
     </row>
     <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
@@ -1642,17 +1686,17 @@
         <f>GEOMEAN(K19:N19)</f>
         <v>2.7355647997347612</v>
       </c>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="37"/>
-      <c r="AA19" s="37"/>
-      <c r="AB19" s="37"/>
-      <c r="AC19" s="37"/>
-      <c r="AD19" s="37"/>
-      <c r="AE19" s="37"/>
-      <c r="AF19" s="37"/>
-      <c r="AG19" s="37"/>
-      <c r="AH19" s="37"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="23"/>
     </row>
     <row r="20" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -1673,6 +1717,10 @@
       <c r="F20" s="1">
         <v>4.2676499999999997</v>
       </c>
+      <c r="G20">
+        <f>SUM(F16:F19)</f>
+        <v>1</v>
+      </c>
       <c r="J20" s="7" t="s">
         <v>6</v>
       </c>
@@ -1691,17 +1739,20 @@
       <c r="O20" s="1">
         <v>4.1486200000000002</v>
       </c>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="37"/>
+      <c r="P20" s="20">
+        <v>1</v>
+      </c>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="23"/>
+      <c r="AH20" s="23"/>
     </row>
     <row r="21" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -1742,17 +1793,17 @@
         <f xml:space="preserve"> (O20 - COUNT(K16:K19)) / (COUNT(K16:K19) - 1)</f>
         <v>4.9540000000000063E-2</v>
       </c>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="37"/>
-      <c r="AC21" s="37"/>
-      <c r="AD21" s="37"/>
-      <c r="AE21" s="37"/>
-      <c r="AF21" s="37"/>
-      <c r="AG21" s="37"/>
-      <c r="AH21" s="37"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
     </row>
     <row r="22" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
@@ -1793,59 +1844,59 @@
         <f>O21/$E$47</f>
         <v>5.5044444444444514E-2</v>
       </c>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="37"/>
-      <c r="AC22" s="37"/>
-      <c r="AD22" s="37"/>
-      <c r="AE22" s="37"/>
-      <c r="AF22" s="37"/>
-      <c r="AG22" s="37"/>
-      <c r="AH22" s="37"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="23"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
-      <c r="AA23" s="37"/>
-      <c r="AB23" s="37"/>
-      <c r="AC23" s="37"/>
-      <c r="AD23" s="37"/>
-      <c r="AE23" s="37"/>
-      <c r="AF23" s="37"/>
-      <c r="AG23" s="37"/>
-      <c r="AH23" s="37"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="23"/>
     </row>
     <row r="24" spans="1:34" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="J24" s="19" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="J24" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="21"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="37"/>
-      <c r="AA24" s="37"/>
-      <c r="AB24" s="37"/>
-      <c r="AC24" s="37"/>
-      <c r="AD24" s="37"/>
-      <c r="AE24" s="37"/>
-      <c r="AF24" s="37"/>
-      <c r="AG24" s="37"/>
-      <c r="AH24" s="37"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
     </row>
     <row r="25" spans="1:34" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
@@ -1884,7 +1935,7 @@
       <c r="O25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AH25" s="37"/>
+      <c r="AH25" s="23"/>
     </row>
     <row r="26" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
@@ -1903,8 +1954,8 @@
         <v>3</v>
       </c>
       <c r="F26" s="12">
-        <f>G16/SUM($G$26:$G$29)</f>
-        <v>0.25873917409746816</v>
+        <f>G26/SUM($G$26:$G$29)</f>
+        <v>0.19148841359807187</v>
       </c>
       <c r="G26">
         <f>GEOMEAN(B26:E26)</f>
@@ -1913,27 +1964,38 @@
       <c r="J26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="31">
-        <v>1</v>
-      </c>
-      <c r="L26" s="31">
+      <c r="K26" s="18">
+        <v>1</v>
+      </c>
+      <c r="L26" s="18">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="18">
         <v>5</v>
       </c>
-      <c r="N26" s="31">
+      <c r="N26" s="18">
         <v>0.33333333333333331</v>
       </c>
       <c r="O26" s="12">
         <f>P26/SUM($P$26:$P$29)</f>
         <v>0.16426154532505152</v>
       </c>
-      <c r="P26" s="34">
+      <c r="P26" s="20">
         <f>GEOMEAN(K26:N26)</f>
         <v>0.86334002137045041</v>
       </c>
-      <c r="AH26" s="37"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
+      <c r="AB26" s="23"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="23"/>
+      <c r="AE26" s="23"/>
+      <c r="AF26" s="23"/>
+      <c r="AG26" s="23"/>
+      <c r="AH26" s="23"/>
     </row>
     <row r="27" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
@@ -1952,8 +2014,8 @@
         <v>1</v>
       </c>
       <c r="F27" s="12">
-        <f>G17/SUM($G$26:$G$29)</f>
-        <v>0.67626028434758334</v>
+        <f>G27/SUM($G$26:$G$29)</f>
+        <v>7.7227068802438903E-2</v>
       </c>
       <c r="G27">
         <f>GEOMEAN(B27:E27)</f>
@@ -1962,27 +2024,38 @@
       <c r="J27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="31">
+      <c r="K27" s="18">
         <v>3</v>
       </c>
-      <c r="L27" s="31">
-        <v>1</v>
-      </c>
-      <c r="M27" s="31">
+      <c r="L27" s="18">
+        <v>1</v>
+      </c>
+      <c r="M27" s="18">
         <v>6</v>
       </c>
-      <c r="N27" s="31">
+      <c r="N27" s="18">
         <v>1</v>
       </c>
       <c r="O27" s="12">
         <f>P27/SUM($P$26:$P$29)</f>
         <v>0.39189719657716698</v>
       </c>
-      <c r="P27" s="34">
+      <c r="P27" s="20">
         <f>GEOMEAN(K27:N27)</f>
         <v>2.0597671439071177</v>
       </c>
-      <c r="AH27" s="37"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="23"/>
     </row>
     <row r="28" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
@@ -2001,8 +2074,8 @@
         <v>7</v>
       </c>
       <c r="F28" s="12">
-        <f>G18/SUM($G$26:$G$29)</f>
-        <v>8.0828563920884375E-2</v>
+        <f>G28/SUM($G$26:$G$29)</f>
+        <v>0.6540574487970503</v>
       </c>
       <c r="G28">
         <f>GEOMEAN(B28:E28)</f>
@@ -2011,27 +2084,38 @@
       <c r="J28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="31">
+      <c r="K28" s="18">
         <v>0.2</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="18">
         <v>0.16666666666666666</v>
       </c>
-      <c r="M28" s="31">
-        <v>1</v>
-      </c>
-      <c r="N28" s="31">
+      <c r="M28" s="18">
+        <v>1</v>
+      </c>
+      <c r="N28" s="18">
         <v>0.16666666666666666</v>
       </c>
       <c r="O28" s="12">
         <f>P28/SUM($P$26:$P$29)</f>
         <v>5.1944061520614614E-2</v>
       </c>
-      <c r="P28" s="34">
+      <c r="P28" s="20">
         <f>GEOMEAN(K28:N28)</f>
         <v>0.27301208627090667</v>
       </c>
-      <c r="AH28" s="37"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="23"/>
+      <c r="AH28" s="23"/>
     </row>
     <row r="29" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
@@ -2050,8 +2134,8 @@
         <v>1</v>
       </c>
       <c r="F29" s="12">
-        <f>G19/SUM($G$26:$G$29)</f>
-        <v>5.2814912750661594E-2</v>
+        <f>G29/SUM($G$26:$G$29)</f>
+        <v>7.7227068802438903E-2</v>
       </c>
       <c r="G29">
         <f>GEOMEAN(B29:E29)</f>
@@ -2060,27 +2144,38 @@
       <c r="J29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="18">
         <v>3</v>
       </c>
-      <c r="L29" s="31">
-        <v>1</v>
-      </c>
-      <c r="M29" s="31">
+      <c r="L29" s="18">
+        <v>1</v>
+      </c>
+      <c r="M29" s="18">
         <v>6</v>
       </c>
-      <c r="N29" s="31">
+      <c r="N29" s="18">
         <v>1</v>
       </c>
       <c r="O29" s="12">
         <f>P29/SUM($P$26:$P$29)</f>
         <v>0.39189719657716698</v>
       </c>
-      <c r="P29" s="34">
+      <c r="P29" s="20">
         <f>GEOMEAN(K29:N29)</f>
         <v>2.0597671439071177</v>
       </c>
-      <c r="AH29" s="37"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="23"/>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="23"/>
+      <c r="AG29" s="23"/>
+      <c r="AH29" s="23"/>
     </row>
     <row r="30" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
@@ -2101,6 +2196,10 @@
       <c r="F30" s="1">
         <v>4.0571400000000004</v>
       </c>
+      <c r="G30">
+        <f>SUM(F26:F29)</f>
+        <v>1</v>
+      </c>
       <c r="J30" s="7" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2218,21 @@
       <c r="O30" s="1">
         <v>4.09762</v>
       </c>
-      <c r="AH30" s="37"/>
+      <c r="P30" s="20">
+        <v>1</v>
+      </c>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+      <c r="AA30" s="23"/>
+      <c r="AB30" s="23"/>
+      <c r="AC30" s="23"/>
+      <c r="AD30" s="23"/>
+      <c r="AE30" s="23"/>
+      <c r="AF30" s="23"/>
+      <c r="AG30" s="23"/>
+      <c r="AH30" s="23"/>
     </row>
     <row r="31" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
@@ -2160,7 +2273,18 @@
         <f xml:space="preserve"> (O30 - COUNT(K26:K29)) / (COUNT(K26:K29) - 1)</f>
         <v>3.2540000000000013E-2</v>
       </c>
-      <c r="AH31" s="37"/>
+      <c r="W31" s="23"/>
+      <c r="X31" s="23"/>
+      <c r="Y31" s="23"/>
+      <c r="Z31" s="23"/>
+      <c r="AA31" s="23"/>
+      <c r="AB31" s="23"/>
+      <c r="AC31" s="23"/>
+      <c r="AD31" s="23"/>
+      <c r="AE31" s="23"/>
+      <c r="AF31" s="23"/>
+      <c r="AG31" s="23"/>
+      <c r="AH31" s="23"/>
     </row>
     <row r="32" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
@@ -2201,61 +2325,64 @@
         <f>O31/$E$47</f>
         <v>3.6155555555555573E-2</v>
       </c>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="37"/>
-      <c r="AB32" s="37"/>
-      <c r="AC32" s="37"/>
-      <c r="AD32" s="37"/>
-      <c r="AE32" s="37"/>
-      <c r="AF32" s="37"/>
-      <c r="AG32" s="37"/>
-      <c r="AH32" s="37"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="23"/>
+      <c r="AG32" s="23"/>
+      <c r="AH32" s="23"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="X33" s="37"/>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
-      <c r="AA33" s="37"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
-      <c r="AD33" s="37"/>
-      <c r="AE33" s="37"/>
-      <c r="AF33" s="37"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" s="37"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+      <c r="AA33" s="23"/>
+      <c r="AB33" s="23"/>
+      <c r="AC33" s="23"/>
+      <c r="AD33" s="23"/>
+      <c r="AE33" s="23"/>
+      <c r="AF33" s="23"/>
+      <c r="AG33" s="23"/>
+      <c r="AH33" s="23"/>
     </row>
     <row r="34" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="J34" s="19" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
+      <c r="J34" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="21"/>
-      <c r="X34" s="37"/>
-      <c r="Y34" s="37"/>
-      <c r="Z34" s="37"/>
-      <c r="AA34" s="37"/>
-      <c r="AB34" s="37"/>
-      <c r="AC34" s="37"/>
-      <c r="AD34" s="37"/>
-      <c r="AE34" s="37"/>
-      <c r="AF34" s="37"/>
-      <c r="AG34" s="37"/>
-      <c r="AH34" s="37"/>
-    </row>
-    <row r="35" spans="1:34" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="27"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
+      <c r="AA34" s="23"/>
+      <c r="AB34" s="23"/>
+      <c r="AC34" s="23"/>
+      <c r="AD34" s="23"/>
+      <c r="AE34" s="23"/>
+      <c r="AF34" s="23"/>
+      <c r="AG34" s="23"/>
+      <c r="AH34" s="23"/>
+    </row>
+    <row r="35" spans="1:34" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -2292,17 +2419,9 @@
       <c r="O35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="37"/>
-      <c r="Y35" s="37"/>
-      <c r="Z35" s="37"/>
-      <c r="AA35" s="37"/>
-      <c r="AB35" s="37"/>
-      <c r="AC35" s="37"/>
-      <c r="AD35" s="37"/>
-      <c r="AE35" s="37"/>
-      <c r="AF35" s="37"/>
-      <c r="AG35" s="37"/>
-      <c r="AH35" s="37"/>
+      <c r="AF35" s="23"/>
+      <c r="AG35" s="23"/>
+      <c r="AH35" s="23"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
@@ -2347,10 +2466,21 @@
         <f>P36/SUM($P$36:$P$39)</f>
         <v>0.17526935412003866</v>
       </c>
-      <c r="P36" s="34">
+      <c r="P36" s="20">
         <f>GEOMEAN(K36:N36)</f>
         <v>0.8408964152537145</v>
       </c>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="23"/>
+      <c r="AG36" s="23"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
@@ -2395,10 +2525,11 @@
         <f>P37/SUM($P$36:$P$39)</f>
         <v>8.9060098576299609E-2</v>
       </c>
-      <c r="P37" s="34">
+      <c r="P37" s="20">
         <f>GEOMEAN(K37:N37)</f>
         <v>0.42728700639623407</v>
       </c>
+      <c r="AG37" s="23"/>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
@@ -2443,10 +2574,21 @@
         <f>P38/SUM($P$36:$P$39)</f>
         <v>0.2478682976649314</v>
       </c>
-      <c r="P38" s="34">
+      <c r="P38" s="20">
         <f>GEOMEAN(K38:N38)</f>
         <v>1.189207115002721</v>
       </c>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="23"/>
+      <c r="AB38" s="23"/>
+      <c r="AC38" s="23"/>
+      <c r="AD38" s="23"/>
+      <c r="AE38" s="23"/>
+      <c r="AF38" s="23"/>
+      <c r="AG38" s="23"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
@@ -2491,10 +2633,11 @@
         <f>P39/SUM($P$36:$P$39)</f>
         <v>0.48780224963873026</v>
       </c>
-      <c r="P39" s="34">
+      <c r="P39" s="20">
         <f>GEOMEAN(K39:N39)</f>
         <v>2.340347319320716</v>
       </c>
+      <c r="AG39" s="23"/>
     </row>
     <row r="40" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
@@ -2515,6 +2658,9 @@
       <c r="F40" s="1">
         <v>4.1551099999999996</v>
       </c>
+      <c r="G40" s="20">
+        <v>1</v>
+      </c>
       <c r="J40" s="7" t="s">
         <v>6</v>
       </c>
@@ -2533,6 +2679,20 @@
       <c r="O40" s="1">
         <v>4.1033999999999997</v>
       </c>
+      <c r="P40" s="20">
+        <v>1</v>
+      </c>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="23"/>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="23"/>
+      <c r="AE40" s="23"/>
+      <c r="AF40" s="23"/>
+      <c r="AG40" s="23"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
@@ -2573,6 +2733,7 @@
         <f xml:space="preserve"> (O40 - COUNT(K36:K39)) / (COUNT(K36:K39) - 1)</f>
         <v>3.4466666666666569E-2</v>
       </c>
+      <c r="AG41" s="23"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
@@ -2613,20 +2774,68 @@
         <f>O41/$E$47</f>
         <v>3.8296296296296189E-2</v>
       </c>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="23"/>
+      <c r="AA42" s="23"/>
+      <c r="AB42" s="23"/>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="23"/>
+      <c r="AE42" s="23"/>
+      <c r="AF42" s="23"/>
+      <c r="AG42" s="23"/>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="23"/>
+      <c r="AA43" s="23"/>
+      <c r="AB43" s="23"/>
+      <c r="AC43" s="23"/>
+      <c r="AD43" s="23"/>
+      <c r="AE43" s="23"/>
+      <c r="AF43" s="23"/>
+      <c r="AG43" s="23"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="23"/>
+      <c r="AA44" s="23"/>
+      <c r="AB44" s="23"/>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="23"/>
+      <c r="AE44" s="23"/>
+      <c r="AF44" s="23"/>
+      <c r="AG44" s="23"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="23"/>
+      <c r="AA45" s="23"/>
+      <c r="AB45" s="23"/>
+      <c r="AC45" s="23"/>
+      <c r="AD45" s="23"/>
+      <c r="AE45" s="23"/>
+      <c r="AF45" s="23"/>
+      <c r="AG45" s="23"/>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -2659,6 +2868,17 @@
       <c r="J46" s="1">
         <v>9</v>
       </c>
+      <c r="W46" s="23"/>
+      <c r="X46" s="23"/>
+      <c r="Y46" s="23"/>
+      <c r="Z46" s="23"/>
+      <c r="AA46" s="23"/>
+      <c r="AB46" s="23"/>
+      <c r="AC46" s="23"/>
+      <c r="AD46" s="23"/>
+      <c r="AE46" s="23"/>
+      <c r="AF46" s="23"/>
+      <c r="AG46" s="23"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -2691,9 +2911,23 @@
       <c r="J47" s="1">
         <v>1.45</v>
       </c>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="23"/>
+      <c r="AA47" s="23"/>
+      <c r="AB47" s="23"/>
+      <c r="AC47" s="23"/>
+      <c r="AD47" s="23"/>
+      <c r="AE47" s="23"/>
+      <c r="AF47" s="23"/>
+      <c r="AG47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="A24:F24"/>
     <mergeCell ref="J24:O24"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="Q14:T14"/>
@@ -2710,9 +2944,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="A24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fixed priorities in second-level comparision
</commit_message>
<xml_diff>
--- a/doc/apartments.xlsx
+++ b/doc/apartments.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="apartments" sheetId="3" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="28">
   <si>
     <t>Индекс согласованности при случайной оценке сравнений</t>
   </si>
@@ -101,9 +104,6 @@
     <t>Наличие удобств</t>
   </si>
   <si>
-    <t>Пльзовательский рейтинг</t>
-  </si>
-  <si>
     <t>Матрица сравнения третьего уровня (расстояние до общественного транспорта)</t>
   </si>
   <si>
@@ -123,6 +123,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +250,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -434,8 +438,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -544,8 +584,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="223">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="6" builtinId="8" hidden="1"/>
@@ -638,6 +684,24 @@
     <cellStyle name="Гиперссылка" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="5" builtinId="9" hidden="1"/>
@@ -731,6 +795,24 @@
     <cellStyle name="Открывавшаяся гиперссылка" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Процентный" xfId="26" builtinId="5"/>
     <cellStyle name="Стиль 1" xfId="1"/>
   </cellStyles>
@@ -745,6 +827,52 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Config"/>
+      <sheetName val="Wilcoxon Table"/>
+      <sheetName val="Mann Table"/>
+      <sheetName val="RSign Table"/>
+      <sheetName val="Runs Table"/>
+      <sheetName val="KS Table"/>
+      <sheetName val="KS2 Table"/>
+      <sheetName val="Lil Table"/>
+      <sheetName val="AD Table"/>
+      <sheetName val="SW Table"/>
+      <sheetName val="Stud. Q Table"/>
+      <sheetName val="Stud. Q Table 2"/>
+      <sheetName val="Sp Rho Table"/>
+      <sheetName val="Ken Tau Table"/>
+      <sheetName val="Durbin Table"/>
+      <sheetName val="Dunnett Table"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="eVALUES"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,10 +1153,12 @@
     <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
     <col min="23" max="23" width="24" customWidth="1"/>
   </cols>
@@ -1057,7 +1187,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>19</v>
@@ -1098,14 +1228,17 @@
       </c>
       <c r="H3" s="34">
         <f t="shared" ref="H3:H8" si="0">GEOMEAN(B3:G3)/SUM($J$3:$J$8)</f>
-        <v>0.11598237204722957</v>
+        <v>0.10760107321498238</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="24">
         <f t="shared" ref="J3:J8" si="1">GEOMEAN(B3:G3)</f>
         <v>0.81818882300002704</v>
       </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="24">
+        <f>PRODUCT(B3:G3)</f>
+        <v>0.30000000000000004</v>
+      </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -1118,6 +1251,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="6">
+        <f>1/C3</f>
         <v>3</v>
       </c>
       <c r="C4" s="6">
@@ -1137,14 +1271,17 @@
       </c>
       <c r="H4" s="35">
         <f t="shared" si="0"/>
-        <v>0.27430369726673426</v>
+        <v>0.25448153621758307</v>
       </c>
       <c r="I4" s="36"/>
       <c r="J4" s="24">
         <f t="shared" si="1"/>
         <v>1.9350545712225413</v>
       </c>
-      <c r="K4" s="24"/>
+      <c r="K4" s="24">
+        <f t="shared" ref="K4:L9" si="2">PRODUCT(B4:G4)</f>
+        <v>52.5</v>
+      </c>
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
@@ -1152,9 +1289,11 @@
         <v>20</v>
       </c>
       <c r="B5" s="6">
+        <f>1/D3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C5" s="6">
+        <f>1/D4</f>
         <v>0.2</v>
       </c>
       <c r="D5" s="6">
@@ -1164,21 +1303,24 @@
         <v>3</v>
       </c>
       <c r="F5" s="6">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
       <c r="H5" s="34">
         <f t="shared" si="0"/>
-        <v>0.14175501887444597</v>
+        <v>7.6908272977309899E-2</v>
       </c>
       <c r="I5" s="34"/>
       <c r="J5" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="24"/>
+        <v>0.58480354764257325</v>
+      </c>
+      <c r="K5" s="41">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
       <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
@@ -1186,12 +1328,15 @@
         <v>19</v>
       </c>
       <c r="B6" s="6">
+        <f>1/E3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C6" s="6">
+        <f>1/E4</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="D6" s="6">
+        <f>1/E5</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E6" s="6">
@@ -1205,14 +1350,17 @@
       </c>
       <c r="H6" s="34">
         <f t="shared" si="0"/>
-        <v>3.9291958666538389E-2</v>
+        <v>3.6452581945096103E-2</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="24">
         <f t="shared" si="1"/>
         <v>0.27718213420958115</v>
       </c>
-      <c r="K6" s="24"/>
+      <c r="K6" s="40">
+        <f t="shared" si="2"/>
+        <v>4.5351473922902491E-4</v>
+      </c>
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:34" ht="30" x14ac:dyDescent="0.2">
@@ -1220,33 +1368,40 @@
         <v>21</v>
       </c>
       <c r="B7" s="6">
+        <f>1/F3</f>
         <v>2</v>
       </c>
       <c r="C7" s="6">
+        <f>1/F4</f>
         <v>1</v>
       </c>
       <c r="D7" s="6">
-        <v>0.2</v>
+        <f>1/F5</f>
+        <v>5</v>
       </c>
       <c r="E7" s="6">
+        <f>1/F6</f>
         <v>7</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
       <c r="G7" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="34">
-        <f t="shared" si="0"/>
-        <v>0.20210869218483324</v>
+        <f>GEOMEAN(B7:G7)/SUM($J$3:$J$8)</f>
+        <v>0.29967538124405729</v>
       </c>
       <c r="I7" s="34"/>
       <c r="J7" s="24">
         <f t="shared" si="1"/>
-        <v>1.4257603983943821</v>
-      </c>
-      <c r="K7" s="24"/>
+        <v>2.278704478832458</v>
+      </c>
+      <c r="K7" s="24">
+        <f>PRODUCT(B7:G7)</f>
+        <v>140</v>
+      </c>
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
@@ -1254,33 +1409,41 @@
         <v>22</v>
       </c>
       <c r="B8" s="6">
+        <f>1/G3</f>
         <v>5</v>
       </c>
       <c r="C8" s="6">
+        <f>1/G4</f>
         <v>2</v>
       </c>
       <c r="D8" s="6">
+        <f>1/G5</f>
         <v>1</v>
       </c>
       <c r="E8" s="6">
+        <f>1/G6</f>
         <v>5</v>
       </c>
       <c r="F8" s="6">
-        <v>0.33333333333333331</v>
+        <f>1/G7</f>
+        <v>0.5</v>
       </c>
       <c r="G8" s="6">
         <v>1</v>
       </c>
       <c r="H8" s="34">
-        <f t="shared" si="0"/>
-        <v>0.22655826096021861</v>
+        <f>GEOMEAN(B8:G8)/SUM($J$3:$J$8)</f>
+        <v>0.22488115440097131</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="24">
         <f t="shared" si="1"/>
-        <v>1.5982380218994845</v>
-      </c>
-      <c r="K8" s="24"/>
+        <v>1.7099759466766968</v>
+      </c>
+      <c r="K8" s="24">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
@@ -1306,13 +1469,18 @@
         <v>9</v>
       </c>
       <c r="H9" s="37">
-        <v>8.1631300000000007</v>
+        <f>[1]!eVALUES(B3:G8)</f>
+        <v>6.7323745865243563</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="23">
         <f>SUM(H3:I8)</f>
         <v>1</v>
       </c>
+      <c r="K9" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -1338,9 +1506,13 @@
       </c>
       <c r="H10" s="37">
         <f xml:space="preserve"> (H9 - COUNT(B3:B8)) / (COUNT(B3:B8) - 1)</f>
-        <v>0.43262600000000012</v>
+        <v>0.14647491730487125</v>
       </c>
       <c r="I10" s="37"/>
+      <c r="J10" s="23">
+        <f>SUM(J3:J8)</f>
+        <v>7.6039095015838774</v>
+      </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -1366,7 +1538,7 @@
       </c>
       <c r="H11" s="38">
         <f>H10/G47</f>
-        <v>0.34889193548387104</v>
+        <v>0.11812493331038004</v>
       </c>
       <c r="I11" s="39"/>
     </row>
@@ -1390,7 +1562,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="27"/>
       <c r="Q14" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
@@ -1440,7 +1612,7 @@
         <v>13</v>
       </c>
       <c r="S15" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T15" s="19" t="s">
         <v>15</v>
@@ -1495,19 +1667,19 @@
       </c>
       <c r="Q16" s="1">
         <f>($F16*$H$3+$O16*$H$4+$F26*$H$6+$O26*$H$7+$F36*$H$5+$O36*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.22544203099177151</v>
+        <v>0.20045206628630571</v>
       </c>
       <c r="R16" s="1">
         <f>($F17*$H$3+$O17*$H$4+$F27*$H$6+$O27*$H$7+$F37*$H$5+$O37*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.21213101206291404</v>
+        <v>0.23309677930372275</v>
       </c>
       <c r="S16" s="1">
         <f>($F18*$H$3+$O18*$H$4+$F28*$H$6+$O28*$H$7+$F38*$H$5+$O38*$H$8) / SUM($H$3:$I$8)</f>
-        <v>0.19767963186356491</v>
+        <v>0.1887434882656685</v>
       </c>
       <c r="T16" s="1">
         <f>($F19*$H$3+$O19*$H$4+$F29*$H$6+$O29*$H$7+$F39*$H$5+$O39*$H$8)/  SUM($H$3:$I$8)</f>
-        <v>0.36474732508174962</v>
+        <v>0.37770766614430312</v>
       </c>
       <c r="X16" s="22"/>
       <c r="Y16" s="23"/>
@@ -1879,7 +2051,7 @@
       <c r="E24" s="26"/>
       <c r="F24" s="27"/>
       <c r="J24" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
@@ -2354,7 +2526,7 @@
     </row>
     <row r="34" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -2362,7 +2534,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="27"/>
       <c r="J34" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K34" s="26"/>
       <c r="L34" s="26"/>
@@ -2925,11 +3097,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="A1:I1"/>
     <mergeCell ref="Q14:T14"/>
     <mergeCell ref="A45:J45"/>
     <mergeCell ref="A34:F34"/>
@@ -2944,6 +3111,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>